<commit_message>
Add content of storytelling with data post
</commit_message>
<xml_diff>
--- a/assets/storytelling_with_data/storytelling_with_data_samples.xlsx
+++ b/assets/storytelling_with_data/storytelling_with_data_samples.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adba\IdeaProjects\adrianbaertschi.github.io\assets\storytelling_with_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB6428E-2E29-49ED-A1B4-A6F8C7836F5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2577AD-ABB8-4412-80D0-ACCECB2AA4A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{310EA8A3-4319-4BD0-B5D4-0F6B09DA3F93}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{310EA8A3-4319-4BD0-B5D4-0F6B09DA3F93}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
+    <sheet name="Lines" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
   <si>
     <t>Category 1</t>
   </si>
@@ -65,7 +66,25 @@
     <t>Metric 3</t>
   </si>
   <si>
-    <t>Sum</t>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -134,6 +153,1254 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Line</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Lines!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-2624-4904-9594-02D278F576B1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-2624-4904-9594-02D278F576B1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-2624-4904-9594-02D278F576B1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-2624-4904-9594-02D278F576B1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{AA21613E-EE55-451A-87F1-5C62820141D8}" type="SERIESNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[SERIES NAME]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-2624-4904-9594-02D278F576B1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Lines!$B$2:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Lines!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>Lines!$A$1:$C$1</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="2">
+                    <c:v>A</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2624-4904-9594-02D278F576B1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Lines!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-2624-4904-9594-02D278F576B1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-2624-4904-9594-02D278F576B1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-2624-4904-9594-02D278F576B1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-2624-4904-9594-02D278F576B1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Lines!$B$2:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Lines!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2624-4904-9594-02D278F576B1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
+        <c:smooth val="0"/>
+        <c:axId val="510228880"/>
+        <c:axId val="510224288"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="510228880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510224288"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="510224288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510228880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="20" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+            <a:alpha val="33000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36BCFA96-8913-4DD6-A482-2565F5A8775A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,7 +1750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A88A31-70A7-4645-95A0-40CC37DE8130}">
   <dimension ref="B2:O18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -539,30 +1806,30 @@
       </c>
       <c r="C3">
         <f ca="1">RANDBETWEEN(1, 20)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:E8" ca="1" si="0">RANDBETWEEN(1, 20)</f>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
         <v>0</v>
       </c>
       <c r="H3">
         <f ca="1">RANDBETWEEN(1, 20)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:J8" ca="1" si="1">RANDBETWEEN(1, 20)</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L3" t="s">
         <v>0</v>
@@ -573,11 +1840,11 @@
       </c>
       <c r="N3">
         <f t="shared" ref="N3:O8" ca="1" si="2">RANDBETWEEN(1, 20)</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="O3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.55000000000000004">
@@ -586,7 +1853,7 @@
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C8" ca="1" si="3">RANDBETWEEN(1, 20)</f>
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
@@ -594,22 +1861,22 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H8" ca="1" si="4">RANDBETWEEN(1, 20)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="L4" t="s">
         <v>1</v>
@@ -620,11 +1887,11 @@
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.55000000000000004">
@@ -633,11 +1900,11 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
@@ -648,15 +1915,15 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L5" t="s">
         <v>2</v>
@@ -667,11 +1934,11 @@
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.55000000000000004">
@@ -680,15 +1947,15 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
         <v>3</v>
@@ -699,7 +1966,7 @@
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="1"/>
@@ -710,15 +1977,15 @@
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.55000000000000004">
@@ -727,45 +1994,45 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="L7" t="s">
         <v>4</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.55000000000000004">
@@ -774,37 +2041,37 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L8" t="s">
         <v>5</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="2"/>
@@ -812,7 +2079,7 @@
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.55000000000000004">
@@ -859,11 +2126,11 @@
       </c>
       <c r="C13">
         <f ca="1">RANDBETWEEN(1, 20)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <f t="shared" ref="D13:E18" ca="1" si="6">RANDBETWEEN(1, 20)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="6"/>
@@ -878,26 +2145,26 @@
       </c>
       <c r="I13">
         <f t="shared" ref="I13:J18" ca="1" si="7">RANDBETWEEN(1, 20)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="7"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L13" t="s">
         <v>0</v>
       </c>
       <c r="M13">
         <f ca="1">RANDBETWEEN(1, 20)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N13">
         <f t="shared" ref="N13:O18" ca="1" si="8">RANDBETWEEN(1, 20)</f>
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="8"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.55000000000000004">
@@ -906,30 +2173,30 @@
       </c>
       <c r="C14">
         <f t="shared" ref="C14:C18" ca="1" si="9">RANDBETWEEN(1, 20)</f>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="6"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G14" t="s">
         <v>1</v>
       </c>
       <c r="H14">
         <f t="shared" ref="H14:H18" ca="1" si="10">RANDBETWEEN(1, 20)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="7"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="7"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L14" t="s">
         <v>1</v>
@@ -940,11 +2207,11 @@
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="8"/>
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.55000000000000004">
@@ -953,15 +2220,15 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="9"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="6"/>
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" t="s">
         <v>2</v>
@@ -972,18 +2239,18 @@
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="7"/>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="L15" t="s">
         <v>2</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="11"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="8"/>
@@ -991,7 +2258,7 @@
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.55000000000000004">
@@ -1000,45 +2267,45 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="9"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="6"/>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="6"/>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G16" t="s">
         <v>3</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="10"/>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="7"/>
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L16" t="s">
         <v>3</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="11"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="8"/>
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.55000000000000004">
@@ -1047,45 +2314,45 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="9"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="6"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="10"/>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="7"/>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="7"/>
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="L17" t="s">
         <v>4</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="11"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.55000000000000004">
@@ -1098,41 +2365,41 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="10"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="7"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="7"/>
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="L18" t="s">
         <v>5</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="11"/>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1185,4 +2452,84 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B778A5-DB20-4F8A-8CA3-FB663168C0F8}">
+  <dimension ref="B1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>83</v>
+      </c>
+      <c r="D5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>